<commit_message>
ancillary files  from SSH set up event
</commit_message>
<xml_diff>
--- a/C2data.xlsx
+++ b/C2data.xlsx
@@ -815,13 +815,13 @@
     <xf numFmtId="166" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -903,11 +903,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="137065216"/>
-        <c:axId val="137067520"/>
+        <c:axId val="24233856"/>
+        <c:axId val="24235392"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="137065216"/>
+        <c:axId val="24233856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -941,7 +941,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="137067520"/>
+        <c:crossAx val="24235392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -950,7 +950,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="137067520"/>
+        <c:axId val="24235392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -984,7 +984,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="137065216"/>
+        <c:crossAx val="24233856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1692,11 +1692,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="131445504"/>
-        <c:axId val="131447040"/>
+        <c:axId val="24488576"/>
+        <c:axId val="24506752"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="131445504"/>
+        <c:axId val="24488576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1731,7 +1731,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="131447040"/>
+        <c:crossAx val="24506752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
@@ -1742,7 +1742,7 @@
         <c:minorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="131447040"/>
+        <c:axId val="24506752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1811,7 +1811,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="131445504"/>
+        <c:crossAx val="24488576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="20"/>
@@ -2521,11 +2521,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="131940736"/>
-        <c:axId val="131942272"/>
+        <c:axId val="142846208"/>
+        <c:axId val="142860288"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="131940736"/>
+        <c:axId val="142846208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2560,7 +2560,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="131942272"/>
+        <c:crossAx val="142860288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
@@ -2571,7 +2571,7 @@
         <c:minorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="131942272"/>
+        <c:axId val="142860288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -2640,7 +2640,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="131940736"/>
+        <c:crossAx val="142846208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="20"/>
@@ -3340,11 +3340,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="132174208"/>
-        <c:axId val="132175744"/>
+        <c:axId val="143186176"/>
+        <c:axId val="143200256"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="132174208"/>
+        <c:axId val="143186176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3379,7 +3379,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="132175744"/>
+        <c:crossAx val="143200256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
@@ -3390,7 +3390,7 @@
         <c:minorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="132175744"/>
+        <c:axId val="143200256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -3459,7 +3459,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="132174208"/>
+        <c:crossAx val="143186176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="20"/>
@@ -4159,11 +4159,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="136134656"/>
-        <c:axId val="136136192"/>
+        <c:axId val="143251328"/>
+        <c:axId val="143252864"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="136134656"/>
+        <c:axId val="143251328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4198,7 +4198,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="136136192"/>
+        <c:crossAx val="143252864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
@@ -4209,7 +4209,7 @@
         <c:minorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="136136192"/>
+        <c:axId val="143252864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4276,7 +4276,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="136134656"/>
+        <c:crossAx val="143251328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4975,11 +4975,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="136182784"/>
-        <c:axId val="136426240"/>
+        <c:axId val="143328384"/>
+        <c:axId val="143329920"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="136182784"/>
+        <c:axId val="143328384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5014,7 +5014,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="136426240"/>
+        <c:crossAx val="143329920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
@@ -5025,7 +5025,7 @@
         <c:minorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="136426240"/>
+        <c:axId val="143329920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -5093,7 +5093,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="136182784"/>
+        <c:crossAx val="143328384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
@@ -5811,11 +5811,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="136718976"/>
-        <c:axId val="137056640"/>
+        <c:axId val="143397632"/>
+        <c:axId val="143399168"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="136718976"/>
+        <c:axId val="143397632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5850,7 +5850,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="137056640"/>
+        <c:crossAx val="143399168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
@@ -5861,7 +5861,7 @@
         <c:minorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="137056640"/>
+        <c:axId val="143399168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5928,7 +5928,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="136718976"/>
+        <c:crossAx val="143397632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6149,11 +6149,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="139144192"/>
-        <c:axId val="139588736"/>
+        <c:axId val="24699264"/>
+        <c:axId val="24701184"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="139144192"/>
+        <c:axId val="24699264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6188,7 +6188,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="139588736"/>
+        <c:crossAx val="24701184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -6198,7 +6198,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="139588736"/>
+        <c:axId val="24701184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20"/>
@@ -6266,7 +6266,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="139144192"/>
+        <c:crossAx val="24699264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6891,11 +6891,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="140731904"/>
-        <c:axId val="140733440"/>
+        <c:axId val="26236800"/>
+        <c:axId val="26238336"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="140731904"/>
+        <c:axId val="26236800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6930,7 +6930,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="140733440"/>
+        <c:crossAx val="26238336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
@@ -6941,7 +6941,7 @@
         <c:minorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="140733440"/>
+        <c:axId val="26238336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -7010,7 +7010,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="140731904"/>
+        <c:crossAx val="26236800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="20"/>
@@ -7637,11 +7637,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="197725184"/>
-        <c:axId val="197928064"/>
+        <c:axId val="141503104"/>
+        <c:axId val="141504896"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="197725184"/>
+        <c:axId val="141503104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7676,7 +7676,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="197928064"/>
+        <c:crossAx val="141504896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
@@ -7685,7 +7685,7 @@
         <c:majorTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="197928064"/>
+        <c:axId val="141504896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -7754,7 +7754,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="197725184"/>
+        <c:crossAx val="141503104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="20"/>
@@ -8120,11 +8120,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="213505920"/>
-        <c:axId val="264088576"/>
+        <c:axId val="141540736"/>
+        <c:axId val="141550720"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="213505920"/>
+        <c:axId val="141540736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8159,7 +8159,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="264088576"/>
+        <c:crossAx val="141550720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
@@ -8170,7 +8170,7 @@
         <c:minorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="264088576"/>
+        <c:axId val="141550720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -8239,7 +8239,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="213505920"/>
+        <c:crossAx val="141540736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="20"/>
@@ -8909,11 +8909,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="285779072"/>
-        <c:axId val="285780992"/>
+        <c:axId val="141606272"/>
+        <c:axId val="141952128"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="285779072"/>
+        <c:axId val="141606272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8948,7 +8948,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="285780992"/>
+        <c:crossAx val="141952128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
@@ -8959,7 +8959,7 @@
         <c:minorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="285780992"/>
+        <c:axId val="141952128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -9028,7 +9028,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="285779072"/>
+        <c:crossAx val="141606272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="20"/>
@@ -9728,11 +9728,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="304215936"/>
-        <c:axId val="304237184"/>
+        <c:axId val="24272256"/>
+        <c:axId val="24286336"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="304215936"/>
+        <c:axId val="24272256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9767,7 +9767,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="304237184"/>
+        <c:crossAx val="24286336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
@@ -9778,7 +9778,7 @@
         <c:minorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="304237184"/>
+        <c:axId val="24286336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -9847,7 +9847,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="304215936"/>
+        <c:crossAx val="24272256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="20"/>
@@ -10547,11 +10547,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="131191936"/>
-        <c:axId val="131193472"/>
+        <c:axId val="246246400"/>
+        <c:axId val="246280960"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="131191936"/>
+        <c:axId val="246246400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10586,7 +10586,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="131193472"/>
+        <c:crossAx val="246280960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
@@ -10597,7 +10597,7 @@
         <c:minorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="131193472"/>
+        <c:axId val="246280960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -10666,7 +10666,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="131191936"/>
+        <c:crossAx val="246246400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="20"/>
@@ -11366,11 +11366,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="131359488"/>
-        <c:axId val="131361024"/>
+        <c:axId val="142006912"/>
+        <c:axId val="142012800"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="131359488"/>
+        <c:axId val="142006912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11405,7 +11405,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="131361024"/>
+        <c:crossAx val="142012800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
@@ -11416,7 +11416,7 @@
         <c:minorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="131361024"/>
+        <c:axId val="142012800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -11485,7 +11485,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="131359488"/>
+        <c:crossAx val="142006912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="20"/>
@@ -18297,23 +18297,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:55" ht="25.2" customHeight="1">
-      <c r="B1" s="63" t="str">
+      <c r="B1" s="61" t="str">
         <f>T(Measures!$A21)</f>
         <v>C2</v>
       </c>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
-      <c r="L1" s="63"/>
-      <c r="M1" s="63"/>
-      <c r="N1" s="63"/>
-      <c r="O1" s="63"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="61"/>
+      <c r="O1" s="61"/>
       <c r="P1" s="30"/>
       <c r="Q1" s="30"/>
       <c r="R1" s="30"/>
@@ -18344,22 +18344,22 @@
     </row>
     <row r="2" spans="1:55" ht="25.2" customHeight="1">
       <c r="B2" s="41"/>
-      <c r="C2" s="61" t="s">
+      <c r="C2" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
       <c r="G2" s="67" t="s">
         <v>13</v>
       </c>
       <c r="H2" s="68"/>
       <c r="I2" s="68"/>
-      <c r="J2" s="61" t="s">
+      <c r="J2" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="62"/>
-      <c r="L2" s="62"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
       <c r="M2" s="67" t="s">
         <v>32</v>
       </c>
@@ -18370,61 +18370,61 @@
       </c>
       <c r="Q2" s="69"/>
       <c r="R2" s="70"/>
-      <c r="S2" s="61" t="s">
+      <c r="S2" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="T2" s="62"/>
-      <c r="U2" s="62"/>
-      <c r="V2" s="61" t="s">
+      <c r="T2" s="63"/>
+      <c r="U2" s="63"/>
+      <c r="V2" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="W2" s="61"/>
-      <c r="X2" s="61"/>
-      <c r="Y2" s="61" t="s">
+      <c r="W2" s="62"/>
+      <c r="X2" s="62"/>
+      <c r="Y2" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="Z2" s="62"/>
-      <c r="AA2" s="62"/>
+      <c r="Z2" s="63"/>
+      <c r="AA2" s="63"/>
       <c r="AB2" s="64" t="s">
         <v>43</v>
       </c>
       <c r="AC2" s="65"/>
       <c r="AD2" s="66"/>
-      <c r="AE2" s="61" t="s">
+      <c r="AE2" s="62" t="s">
         <v>27</v>
       </c>
-      <c r="AF2" s="62"/>
-      <c r="AG2" s="62"/>
-      <c r="AH2" s="61" t="s">
+      <c r="AF2" s="63"/>
+      <c r="AG2" s="63"/>
+      <c r="AH2" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="AI2" s="62"/>
-      <c r="AJ2" s="62"/>
-      <c r="AK2" s="61" t="s">
+      <c r="AI2" s="63"/>
+      <c r="AJ2" s="63"/>
+      <c r="AK2" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="AL2" s="62"/>
-      <c r="AM2" s="62"/>
-      <c r="AN2" s="61" t="s">
+      <c r="AL2" s="63"/>
+      <c r="AM2" s="63"/>
+      <c r="AN2" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="AO2" s="61"/>
-      <c r="AP2" s="61"/>
-      <c r="AQ2" s="62" t="s">
+      <c r="AO2" s="62"/>
+      <c r="AP2" s="62"/>
+      <c r="AQ2" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="AR2" s="62"/>
-      <c r="AS2" s="62"/>
-      <c r="AT2" s="62"/>
-      <c r="AU2" s="62"/>
-      <c r="AV2" s="62"/>
-      <c r="AW2" s="62"/>
-      <c r="AX2" s="62"/>
-      <c r="AY2" s="62"/>
-      <c r="AZ2" s="62"/>
-      <c r="BA2" s="62"/>
-      <c r="BB2" s="62"/>
-      <c r="BC2" s="62"/>
+      <c r="AR2" s="63"/>
+      <c r="AS2" s="63"/>
+      <c r="AT2" s="63"/>
+      <c r="AU2" s="63"/>
+      <c r="AV2" s="63"/>
+      <c r="AW2" s="63"/>
+      <c r="AX2" s="63"/>
+      <c r="AY2" s="63"/>
+      <c r="AZ2" s="63"/>
+      <c r="BA2" s="63"/>
+      <c r="BB2" s="63"/>
+      <c r="BC2" s="63"/>
     </row>
     <row r="3" spans="1:55" s="56" customFormat="1" ht="180" customHeight="1">
       <c r="A3" s="12" t="s">
@@ -19515,14 +19515,14 @@
       </c>
       <c r="J9" s="19">
         <f ca="1">0.1*RANDBETWEEN(4,8)*H9</f>
-        <v>32</v>
+        <v>25.6</v>
       </c>
       <c r="K9" s="25">
         <v>64</v>
       </c>
       <c r="L9" s="24">
         <f t="shared" ca="1" si="6"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="M9" s="26"/>
       <c r="N9" s="26"/>
@@ -19669,14 +19669,14 @@
       </c>
       <c r="J10" s="19">
         <f t="shared" ref="J10:J16" ca="1" si="16">0.1*RANDBETWEEN(4,8)*K10</f>
-        <v>27.300000000000004</v>
+        <v>19.5</v>
       </c>
       <c r="K10" s="25">
         <v>39</v>
       </c>
       <c r="L10" s="24">
         <f t="shared" ca="1" si="6"/>
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="M10" s="26"/>
       <c r="N10" s="26"/>
@@ -19823,14 +19823,14 @@
       </c>
       <c r="J11" s="19">
         <f t="shared" ca="1" si="16"/>
-        <v>35.200000000000003</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="K11" s="25">
         <v>44</v>
       </c>
       <c r="L11" s="24">
         <f t="shared" ca="1" si="6"/>
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="M11" s="26"/>
       <c r="N11" s="26"/>
@@ -19977,14 +19977,14 @@
       </c>
       <c r="J12" s="19">
         <f t="shared" ca="1" si="16"/>
-        <v>32.400000000000006</v>
+        <v>27</v>
       </c>
       <c r="K12" s="25">
         <v>54</v>
       </c>
       <c r="L12" s="24">
         <f t="shared" ca="1" si="6"/>
-        <v>60.000000000000007</v>
+        <v>50</v>
       </c>
       <c r="M12" s="26"/>
       <c r="N12" s="26"/>
@@ -20131,14 +20131,14 @@
       </c>
       <c r="J13" s="19">
         <f t="shared" ca="1" si="16"/>
-        <v>19.200000000000003</v>
+        <v>22.400000000000002</v>
       </c>
       <c r="K13" s="25">
         <v>32</v>
       </c>
       <c r="L13" s="24">
         <f t="shared" ca="1" si="6"/>
-        <v>60.000000000000007</v>
+        <v>70</v>
       </c>
       <c r="M13" s="26"/>
       <c r="N13" s="26"/>
@@ -20285,14 +20285,14 @@
       </c>
       <c r="J14" s="19">
         <f t="shared" ca="1" si="16"/>
-        <v>35.700000000000003</v>
+        <v>40.800000000000004</v>
       </c>
       <c r="K14" s="25">
         <v>51</v>
       </c>
       <c r="L14" s="24">
         <f t="shared" ca="1" si="6"/>
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="M14" s="26"/>
       <c r="N14" s="26"/>
@@ -20439,14 +20439,14 @@
       </c>
       <c r="J15" s="19">
         <f t="shared" ca="1" si="16"/>
-        <v>29.400000000000006</v>
+        <v>24.5</v>
       </c>
       <c r="K15" s="25">
         <v>49</v>
       </c>
       <c r="L15" s="24">
         <f t="shared" ca="1" si="6"/>
-        <v>60.000000000000007</v>
+        <v>50</v>
       </c>
       <c r="M15" s="26"/>
       <c r="N15" s="26"/>
@@ -20593,14 +20593,14 @@
       </c>
       <c r="J16" s="19">
         <f t="shared" ca="1" si="16"/>
-        <v>26</v>
+        <v>31.200000000000003</v>
       </c>
       <c r="K16" s="25">
         <v>52</v>
       </c>
       <c r="L16" s="24">
         <f t="shared" ca="1" si="6"/>
-        <v>50</v>
+        <v>60.000000000000007</v>
       </c>
       <c r="M16" s="26"/>
       <c r="N16" s="26"/>
@@ -24200,6 +24200,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="AE2:AG2"/>
+    <mergeCell ref="AH2:AJ2"/>
+    <mergeCell ref="AK2:AM2"/>
+    <mergeCell ref="AN2:AP2"/>
+    <mergeCell ref="AQ2:BC2"/>
     <mergeCell ref="B1:O1"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="AB2:AD2"/>
@@ -24210,11 +24215,6 @@
     <mergeCell ref="V2:X2"/>
     <mergeCell ref="Y2:AA2"/>
     <mergeCell ref="P2:R2"/>
-    <mergeCell ref="AE2:AG2"/>
-    <mergeCell ref="AH2:AJ2"/>
-    <mergeCell ref="AK2:AM2"/>
-    <mergeCell ref="AN2:AP2"/>
-    <mergeCell ref="AQ2:BC2"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="6">
@@ -24281,19 +24281,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="22.2" customHeight="1">
-      <c r="A1" s="63" t="str">
+      <c r="A1" s="61" t="str">
         <f>T(Measures!$A21)</f>
         <v>C2</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
     </row>
     <row r="2" spans="1:22" s="2" customFormat="1" ht="13.5" customHeight="1">
       <c r="S2" s="3"/>
@@ -24395,19 +24395,19 @@
   <sheetFormatPr defaultRowHeight="13.2"/>
   <sheetData>
     <row r="1" spans="1:10" ht="27" customHeight="1">
-      <c r="A1" s="63" t="str">
+      <c r="A1" s="61" t="str">
         <f>T(Measures!A21)</f>
         <v>C2</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
     </row>
     <row r="5" spans="1:10" ht="12.75" customHeight="1"/>
     <row r="38" ht="12.75" customHeight="1"/>
@@ -24437,19 +24437,19 @@
   <sheetFormatPr defaultRowHeight="13.2"/>
   <sheetData>
     <row r="1" spans="1:10" ht="27" customHeight="1">
-      <c r="A1" s="63" t="str">
+      <c r="A1" s="61" t="str">
         <f>T(Measures!A21)</f>
         <v>C2</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
     </row>
     <row r="5" spans="1:10" ht="12.75" customHeight="1"/>
     <row r="38" ht="12.75" customHeight="1"/>

</xml_diff>